<commit_message>
Added efficiency parameters. Increased to hourly step size for CA test instance.
</commit_message>
<xml_diff>
--- a/evrp/data/parameters.xlsx
+++ b/evrp/data/parameters.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,15 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ramiariss/PycharmProjects/e-vrp/evrp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{5BD10262-8EDC-5C40-B064-6255B246BAFF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3458FD4-132B-2D47-BE3C-8BAAF85008BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3220" yWindow="-21620" windowWidth="27640" windowHeight="16940" activeTab="1"/>
+    <workbookView xWindow="-3220" yWindow="-21620" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vehicle_parameters" sheetId="1" r:id="rId1"/>
     <sheet name="energy_prices" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -264,7 +275,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.000_);[Red]\(&quot;$&quot;#,##0.000\)"/>
@@ -1296,11 +1307,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1524,25 +1535,25 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D4" r:id="rId3"/>
-    <hyperlink ref="D10" r:id="rId4"/>
-    <hyperlink ref="D11" r:id="rId5"/>
-    <hyperlink ref="D8" r:id="rId6"/>
-    <hyperlink ref="D5" r:id="rId7"/>
-    <hyperlink ref="D6" r:id="rId8"/>
-    <hyperlink ref="D7" r:id="rId9"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D10" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D11" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="D5" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="D6" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="D7" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AP1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
+    <sheetView topLeftCell="S1" workbookViewId="0">
       <selection activeCell="AO18" sqref="AO18"/>
     </sheetView>
   </sheetViews>
@@ -2574,7 +2585,7 @@
         <v>16</v>
       </c>
       <c r="AN17" s="6">
-        <f t="shared" ref="AN17:AN19" si="2">AM17/$B$1</f>
+        <f t="shared" ref="AN17:AN18" si="2">AM17/$B$1</f>
         <v>64</v>
       </c>
       <c r="AO17" s="6">
@@ -30762,19 +30773,19 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" display="https://library.sce.com/?10000_group.propertyvalues.property=jcr%3Acontent%2Fmetadata%2Fcq%3Atags&amp;10000_group.propertyvalues.operation=equals&amp;10000_group.propertyvalues.0_values=sce-document-library%3Aregulatory%2Fsce-tariff-books%2Felectric%2Fschedules%2Fgeneral-service-%26-industrial-rates"/>
-    <hyperlink ref="B9" r:id="rId2" display="https://library.sce.com/content/dam/sce-doclib/public/regulatory/tariff/electric/schedules/general-service-&amp;-industrial-rates/ELECTRIC_SCHEDULES_GS-1.pdf"/>
-    <hyperlink ref="F9" r:id="rId3" display="https://library.sce.com/content/dam/sce-doclib/public/regulatory/tariff/electric/schedules/general-service-&amp;-industrial-rates/ELECTRIC_SCHEDULES_TOU-GS-1.pdf"/>
-    <hyperlink ref="J9" r:id="rId4" display="https://library.sce.com/content/dam/sce-doclib/public/regulatory/tariff/electric/schedules/general-service-&amp;-industrial-rates/ELECTRIC_SCHEDULES_TOU-GS-1.pdf"/>
-    <hyperlink ref="N9" r:id="rId5" display="https://library.sce.com/content/dam/sce-doclib/public/regulatory/tariff/electric/schedules/general-service-&amp;-industrial-rates/ELECTRIC_SCHEDULES_TOU-GS-1-RTP.pdf"/>
-    <hyperlink ref="R9" r:id="rId6" display="https://library.sce.com/content/dam/sce-doclib/public/regulatory/tariff/electric/schedules/general-service-&amp;-industrial-rates/ELECTRIC_SCHEDULES_TOU-GS-1.pdf"/>
-    <hyperlink ref="V9" r:id="rId7" display="https://library.sce.com/content/dam/sce-doclib/public/regulatory/tariff/electric/schedules/general-service-&amp;-industrial-rates/ELECTRIC_SCHEDULES_TOU-GS-1.pdf"/>
-    <hyperlink ref="Z9" r:id="rId8" display="https://library.sce.com/content/dam/sce-doclib/public/regulatory/tariff/electric/schedules/general-service-&amp;-industrial-rates/ELECTRIC_SCHEDULES_TOU-EV-8.pdf"/>
-    <hyperlink ref="AE5" r:id="rId9"/>
-    <hyperlink ref="AE9" r:id="rId10"/>
-    <hyperlink ref="AI9" r:id="rId11"/>
-    <hyperlink ref="AN5" r:id="rId12"/>
-    <hyperlink ref="AN9" r:id="rId13"/>
+    <hyperlink ref="B5" r:id="rId1" display="https://library.sce.com/?10000_group.propertyvalues.property=jcr%3Acontent%2Fmetadata%2Fcq%3Atags&amp;10000_group.propertyvalues.operation=equals&amp;10000_group.propertyvalues.0_values=sce-document-library%3Aregulatory%2Fsce-tariff-books%2Felectric%2Fschedules%2Fgeneral-service-%26-industrial-rates" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="B9" r:id="rId2" display="https://library.sce.com/content/dam/sce-doclib/public/regulatory/tariff/electric/schedules/general-service-&amp;-industrial-rates/ELECTRIC_SCHEDULES_GS-1.pdf" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="F9" r:id="rId3" display="https://library.sce.com/content/dam/sce-doclib/public/regulatory/tariff/electric/schedules/general-service-&amp;-industrial-rates/ELECTRIC_SCHEDULES_TOU-GS-1.pdf" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="J9" r:id="rId4" display="https://library.sce.com/content/dam/sce-doclib/public/regulatory/tariff/electric/schedules/general-service-&amp;-industrial-rates/ELECTRIC_SCHEDULES_TOU-GS-1.pdf" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="N9" r:id="rId5" display="https://library.sce.com/content/dam/sce-doclib/public/regulatory/tariff/electric/schedules/general-service-&amp;-industrial-rates/ELECTRIC_SCHEDULES_TOU-GS-1-RTP.pdf" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="R9" r:id="rId6" display="https://library.sce.com/content/dam/sce-doclib/public/regulatory/tariff/electric/schedules/general-service-&amp;-industrial-rates/ELECTRIC_SCHEDULES_TOU-GS-1.pdf" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="V9" r:id="rId7" display="https://library.sce.com/content/dam/sce-doclib/public/regulatory/tariff/electric/schedules/general-service-&amp;-industrial-rates/ELECTRIC_SCHEDULES_TOU-GS-1.pdf" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="Z9" r:id="rId8" display="https://library.sce.com/content/dam/sce-doclib/public/regulatory/tariff/electric/schedules/general-service-&amp;-industrial-rates/ELECTRIC_SCHEDULES_TOU-EV-8.pdf" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="AE5" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="AE9" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="AI9" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="AN5" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="AN9" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId14"/>

</xml_diff>